<commit_message>
Various updates: Internal functions 'internalized' New vignette
</commit_message>
<xml_diff>
--- a/inst/shiny/seqNdisplayR_arguments.xlsx
+++ b/inst/shiny/seqNdisplayR_arguments.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au530301_uni_au_dk/Documents/Vedhæftede filer/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/shiny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{FC8B2EBB-2791-4145-ADF8-14C890E04D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E8664BC-1343-8E41-B3BF-C254FFF9475B}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="8_{FC8B2EBB-2791-4145-ADF8-14C890E04D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D6DE3F4-753F-C64A-8F88-C2F965464017}"/>
   <bookViews>
-    <workbookView xWindow="51340" yWindow="500" windowWidth="41000" windowHeight="24760" xr2:uid="{CB5AA8F4-A4C2-334C-ABF2-45A658C283DC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22300" activeTab="7" xr2:uid="{CB5AA8F4-A4C2-334C-ABF2-45A658C283DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ExamplesSampleSheetsFolder" sheetId="2" r:id="rId1"/>
+    <sheet name="ListExamplesSampleSheets" sheetId="3" r:id="rId2"/>
+    <sheet name="LoadExcel" sheetId="4" r:id="rId3"/>
+    <sheet name="LoadIGVSession" sheetId="5" r:id="rId4"/>
+    <sheet name="Seesion2xlsx" sheetId="6" r:id="rId5"/>
+    <sheet name="run_seqNdisplayR_app" sheetId="7" r:id="rId6"/>
+    <sheet name="SeqNdisplay" sheetId="1" r:id="rId7"/>
+    <sheet name="seqNdisplayRsession" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="221">
   <si>
     <t>ARGUMENT</t>
   </si>
@@ -330,9 +337,6 @@
   </si>
   <si>
     <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>c("#C1B49A", #F1F1F2)</t>
   </si>
   <si>
     <t>c(100, 100)</t>
@@ -970,6 +974,399 @@
 bigwigs[["-"]] = { "treatment-timeseries" = { "condition 1"= { t0=c("c1t0minus_rep1", "c1t0minus_rep2"), t1=c("c1t1minus_rep1", "c1t1minus_rep2"), …, tT=c("c1tTminus_rep1", "c1tTminus_rep2") }, "condition 2"= { t0=c("c2t0minus_rep1", "c2t0minus_rep2"), t1=c("c2t1minus_rep1", "c2t1minus_rep2"), …, tT=c("c2tTminus_rep1", "c2tTminus_rep2") }, ..., "condition C"= { t0=c("C2t0minus_rep1", "cCt0minus_rep2"), t1=c("cCt1minus_rep1", "cCt1minus_rep2"), …, tT=c("cCtTminus_rep1", "cCtTminus_rep2") } }, 
                    "RNA-seq" = { "condition 1"=c("c1minus_rep1", "c1minus_rep2", "c1minus_rep3"), "condition 2"=c("c2minus_rep1", "c2minus_rep2", "c2minus_rep3"), ..., "condition C"=c("cCminus_rep1", "cCminus_rep2", "cCminus_rep3") } }</t>
     </r>
+  </si>
+  <si>
+    <t>Not sure of how the curent internal format is for plus and minus strand (is it a list?)</t>
+  </si>
+  <si>
+    <t>Vector specifying the wanted vertical order of the plot elements (header, scale, names of individual datasets, annotations, unstranded-beds, thickline-spacer, line-spacer and empty-spacer)
+Example:
+c("header","scale","RNA-seq","line-spacer","TT-seq","emptys-spacer","thickline-spacer","annotatation1","unstranded-bedX","annotation2")</t>
+  </si>
+  <si>
+    <t>I remember this was to preload tracks to plot faster (but with some limitaion on the annotation maybe?), but I could not remember the format (TURE FALSE?) or even find back any place where I would have used it in the old files</t>
+  </si>
+  <si>
+    <t>Nested List</t>
+  </si>
+  <si>
+    <t>Vector / List ?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>LOGI</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Logical vector</t>
+  </si>
+  <si>
+    <t>NUM</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>Num vector / list</t>
+  </si>
+  <si>
+    <t>Logical, if TRUE, returns the list of tracks used rather plotting</t>
+  </si>
+  <si>
+    <t>Logical, if TRUE, returns the list of plotting parameters rather plotting</t>
+  </si>
+  <si>
+    <t>Logical, defining whether both strands should be displayed ("TRUE") or only the strand of the feature of interest ("FALSE")</t>
+  </si>
+  <si>
+    <t>Logical, defining whether when displaying both strands separately, negative tracks data should be represented as negative values ("TRUE") or positive ones ("FALSE")</t>
+  </si>
+  <si>
+    <t>Logical, defining whether when displaying both strands, their representation should be interingled ("TRUE") or separated ("FALSE")</t>
+  </si>
+  <si>
+    <t>Logical, defining whether the display of a negative strand feature should be mirrored ("TRUE") to be visualised from left to right or not ("FALSE"). Doing so slows down plotting</t>
+  </si>
+  <si>
+    <t>Logical, defining whether successive datasets should be displayed on different background colors ("TRUE") or not ("FALSE")</t>
+  </si>
+  <si>
+    <t>c("#C1B49A", "#F1F1F2")</t>
+  </si>
+  <si>
+    <t>Vetcor containing two color values as text or hex code.
+Example:
+c("red","blue")
+c("#C1B49A", "#F1F1F2")
+c("red", "#F1F1F2")</t>
+  </si>
+  <si>
+    <t>Numerical value defining the apha value for the background colors</t>
+  </si>
+  <si>
+    <t>Isn't the default c(100,50) ? At least that's what iti is in shiny</t>
+  </si>
+  <si>
+    <t>Numerical vector containing two values corresponding to the alpha for the Plus and Minus strand colors respectively</t>
+  </si>
+  <si>
+    <t>Defines the type of color to use for the Minus strand when intermingled display is used. Can be:
+"same" : similar color as for the Plus strand
+"complementary" : complementary color as compared to the Plus strand (as defined by the XXXXX package)
+"analogous_right" : analogous right color as compared to the Plus strand (as defined by the XXXXX package)
+"analogous_left" : analogous left color as compared to the Plus strand (as defined by the XXXXX package)</t>
+  </si>
+  <si>
+    <t>Name of the locus to plot (case must match annotation)
+Example:
+c("LMO4")
+c("Sox17")</t>
+  </si>
+  <si>
+    <t>Coordinates to plot (when no 'feature' is specified), as  &lt;chromosome&gt;:&lt;strand&gt;:&lt;start&gt;:&lt;end&gt;
+Accepts commas in the coordinates and dashes in between &lt;start&gt; and &lt;end&gt;
+If no strand is specified, Plus strand will be plotted by default
+Example:
+c("chr1:+:87325400:87351991")
+c("chr1:87,326,880-87,350,923")</t>
+  </si>
+  <si>
+    <t>Numerical vector containing two values corresponding to the proportion of the feature length to plot upstream and downstream respectively (only when 'feature' is specified)
+Example:
+c(1,1.5)   will plot the same length as the locus of interest upsream of it and one and half time its length downstream</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Nested list providing for each dataset the information relative to the type of plotting to perform. Associated parameters are:
+bin_stats: type of bining statistic to use for bining. Can be c("mean","median","max")
+enhance_signals: whether signal enhancement should be used. "TRUE" or "FALSE"
+log2transform: whether log2 transformation should be applied. "TRUE" or "FALSE"
+pseudoCount: value of pseudoCount to use upon Log2 transformation (numerical)
+batchCorrect: whether batch correction should be applied (will include samples not displayed). "TRUE" or "FALSE"
+batch: vector specifying the order of samples batched
+whichReps: vector or named nested list specifying replicates to plots. Can only be used if bw file names include their replicate number under the form "_rep1_", "_rep2_",..., the replicates to plot can be specified ("NULL" will plot all replicates) under the form "c(1,2)" if the full set of replicates has to be plotted, otherwise a detailed list of replicates to plot has to be given as a named nested list of similar structure as the dataset as
+            { "treatment-timeseries" = { "condition 1"= { t0=c(1), t1=c(2), …, tT=c(X) }, "condition 2"= { t0=c(2), t1=c(1), …, tT=c(X) }}
+negative_valued_bw: specify whether the negative strand bw files have negative values. "TRUE" or "FALSE"
+calcMean: specify wether Mean of replicates should be displayed ("TRUE") or if individual replicates should be plotted ("FALSE"). "TRUE" or "FALSE"
+negValsSet0: specify whether negative values should be set to zero. "TRUE" or "FALSE"
+force_scale: define if wanted a maximum scale value for the dataset. Either "NULL" or INT
+group_autoscale: specify whether all tracks from the dataset should be scaled together ("TRUE") or individually ("FALSE"). "TRUE" or "FALSE"
+whichSamples:  nested list of samples to plot ("NULL" will plot all samples)
+Example:
+"RNA-seq"={ "bin_stats"=c("mean"), "enhance_signal"=FALSE, "log2transform"=TRUE, "pseudoCount"=c(1), "batchCorrect"=TRUE, "batch"=c(1,2,3,1,2,3), "whichReps"=NULL, "negative_valued_bw"=FALSE, "calcMean"=TRUE, "negValsSet0"=TRUE, "force_scale"=NULL, "group_autoscale"=TRUE, "whichSamples"=NULL }
+"TT-seq"={ "bin_stats"=c("mean"), "enhance_signal"=TRUE, "log2transform"=TRUE, "pseudoCount"=c(1), "batchCorrect"=TRUE, "batch"=c(1,2,3,1,2,3), "whichReps"=c(1), "negative_valued_bw"=FALSE, "calcMean"=TRUE, "negValsSet0"=TRUE, "force_scale"=c(20), "group_autoscale"=TRUE, "whichSamples"={ "condition 1"= { t0=c("c1t0plus_rep1", "c1t0plus_rep2"), t1=c("c1t1plus_rep1", "c1t1plus_rep2"), …, tT=c("c1tTplus_rep1", "c1tTplus_rep2") }, "condition 2"= { t0=c("c2t0plus_rep1", "c2t0plus_rep2"), t1=c("c2t1plus_rep1", "c2t1plus_rep2"), …, tT=c("c2tTplus_rep1", "c2tTplus_rep2") }, ..., "condition C"= { t0=c("C2t0plus_rep1", "cCt0plus_rep2"), t1=c("cCt1plus_rep1", "cCt1plus_rep2"), …, tT=c("cCtTplus_rep1", "cCtTplus_rep2") } } }
+"ChIP-seq"={ "bin_stats"=c("mean"), "enhance_signal"=TRUE, "log2transform"=TRUE, "pseudoCount"=c(1), "batchCorrect"=TRUE, "batch"=c(1,2,3,1,2,3), "whichReps"={ "treatment-timeseries" = { "condition 1"= { t0=c(1), t1=c(2), …, tT=c(X) }, "condition 2"= { t0=c(2), t1=c(1), …, tT=c(X) }}, "negative_valued_bw"=FALSE, "calcMean"=TRUE, "negValsSet0"=TRUE, "force_scale"=c(20), "group_autoscale"=TRUE, "whichSamples"=NULL }</t>
+  </si>
+  <si>
+    <t>Named list providing information relative to the genome annotation bed files and how to display them. Associated parameters are:
+annotation_file : the full path to access the file
+incl_feature_names : Logical defining whether features names should be writen ("TRUE") or not ("FALSE") upon plotting.
+feature_names_above : Logical defining whether features names upon display should be writen above ("TRUE") or below ("FALSE") their visual representation.
+incl_feature_brackets : Logical defining whether arrows hilighting features position should be displayed ("TRUE") or not ("FALSE").
+incl_feature_shadings : Logical defining whether alternative color shadings hilighting features position should be displayed ("TRUE") or not ("FALSE").
+annotation_packing : Parameter indicating the level of visual compaction of features wanted for the annotation. Can be: "expanded" (displays all variants of each feature with individual naming), "squished" (displays all variants of each feature under a common naming), "collapsed" (regroup all overlapping features into one), or "collapsed2" (regroup all variants of a unique features into one, but without merging independen features)
+annot_cols : color wanted for the annotation display as text or hex
+Example:
+"in-house"=list { "annotation_file"=c("http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/annotations/HeLa_major_isoform_hg38_gc34.bed"), "incl_feature_names"=TRUE, "feature_names_above"=TRUE, "incl_feature_brackets"= TRUE, "incl_feature_shadings"=TRUE, "annotation_packing"=c("collapsed2"), "annot_cols"=c("#000000") }</t>
+  </si>
+  <si>
+    <t>Check that this has not evolved based on the 4 following arguments</t>
+  </si>
+  <si>
+    <t>Named vector specifying for each annotation the requested level of compaction.  Can be: "expanded" (displays all variants of each feature with individual naming), "squished" (displays all variants of each feature under a common naming), "collapsed" (regroup all overlapping features into one), or "collapsed2" (regroup all variants of a unique features into one, but without merging independen features)
+Example:
+c{ "RNA-seq"=c("collpased"), "TT-seq"=c("collpased2") }</t>
+  </si>
+  <si>
+    <t>Named vector specifying for each annotation the requested color to use for display of features as text or hex
+Example:
+c{ "RNA-seq"=c("red"), "TT-seq"=c("#000000") }</t>
+  </si>
+  <si>
+    <t>Color as text or hex to use for the annotations names</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the size of the annotation names displays</t>
+  </si>
+  <si>
+    <t>Numerical values specifying at which poisition of the display binning should be initiated</t>
+  </si>
+  <si>
+    <t>I actually could never text this prperly (like the function plots but I canot see any visual difference)</t>
+  </si>
+  <si>
+    <t>Integer value specifying the wanted bin size</t>
+  </si>
+  <si>
+    <t>Integer value specifying the number of bins to display per cm</t>
+  </si>
+  <si>
+    <t>We need to make a schematic of argument priorities: like if I remember correctly, this one gets overrulled if you specify both bin_size AND plot width in cm</t>
+  </si>
+  <si>
+    <t>Applies to the full  function: we need to make a list of all the mandatory arguments vs optionals</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted height of the full plot in cm</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted heigth for each sequencing tracks in cm</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted heigth for the title field in cm</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted heigth for the genomic scale in cm</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted heigth for all annotations tracks together in cm</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted heigth for each dataset spacer in cm</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted maximum width for the datasets naming panel in cm</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted width for all sequencing tracks (excluding all labels) in cm</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted width of the full plot in cm</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the wanted widthfor the margin between sequencing tracks and labels in cm</t>
+  </si>
+  <si>
+    <t>Logical value specifying if all the space defined using panels_max_width_cm should be used for the labels (TRUE) or if they can take less space when possible (FALSE)</t>
+  </si>
+  <si>
+    <t>Named logical vectors list containing one verctor per dataset. Each vector has to be of similar length as the number of subgroup it possess and specify if the legend should be displayed horizontaly (TRUE) or verctically (FALSE)
+Example:
+c{"RNA-seq"=c(TRUE,TRUE), "3P-seq"=c(TRUE,TRUE,FALSE)}</t>
+  </si>
+  <si>
+    <t>Vector list</t>
+  </si>
+  <si>
+    <t>Can be a numerical, a named vector or a named vector list specifying the font size to use for labels names. A numerical will set the value for all labels, a named vector can be used to set independent values for all labels for each datsets and a named vector list can be used to set values for each level of labeling individually. In this later case, each vector should be of length similar to the level of substting in each dataset 
+Example:
+c(5)
+c("RNA-seq"=5, "TT-seq"=6)
+c{  "RNA-seq"=c(5,4), "3P-seq"=c(6,5,4)  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vector specifying two colors as text or hex to use for the datasets labels (first color) and all subsequent labels (second color)
+Example:
+c("red","blue")
+c("red","#000000")
+c("#000000","#000000") </t>
+  </si>
+  <si>
+    <t>Logical value specifying whether horizontal lines separating datsets dataset should be displayed (TRUE) or not (FALSE)</t>
+  </si>
+  <si>
+    <t>Logical vector of length 2, specifying whether vertical lines highlighting replicates belonging to a similar sample (first value) and samples belonging to a similar dataset (second value) should be displayed (TRUE) or not (FALSE)</t>
+  </si>
+  <si>
+    <t>Numerical vector of lengt 3, specifing the weight of the three types of separators. Values one and two refer to the vertical spearators and value three to the horizontal one.</t>
+  </si>
+  <si>
+    <t>Vector of either one or three color(s) as text or hex specifying which hue to use for all separators (when only one value is provided) or for each type individually (Values one and two refer to the vertical spearators and value three to the horizontal one).
+Example:
+c("black")
+c("blue", "#000000", "red")</t>
+  </si>
+  <si>
+    <t>I know these got split for the shiny app and I guess the first one only take one numerical while the second one takes the two other possibilites but since I am not 100% sure I leave it like this for now</t>
+  </si>
+  <si>
+    <t>Logical value specifying whether the datasets names shoudl be displayed (TRUE) or not (FALSE).</t>
+  </si>
+  <si>
+    <t>Logical value specifying if tracks labels should be dislayed as one line reporting all subgroups names separated by a dot (TRUE) or not (FALSE).</t>
+  </si>
+  <si>
+    <t>Character vector specifying the prefix to use for replicates labels</t>
+  </si>
+  <si>
+    <t>Can be a single logical (applyig to all datasets) or a named logical vector reproting for each dataset whether group autoscaling should be applied (TRUE) or not (FALSE).</t>
+  </si>
+  <si>
+    <t>Logical specifying whether the scale of the tracks should be displayed or not</t>
+  </si>
+  <si>
+    <t>Argument specifiying whether scientificnumerotation can ("allow"), has too ("all") or should not ("none") be used for the tracks scales</t>
+  </si>
+  <si>
+    <t>Named numerical vector list</t>
+  </si>
+  <si>
+    <t>Either NULL or a list of named numerical vectors of 2 values. NULL will autoscale all datasets. The list hast to provide for each datasets where manual scaling is required (autoscalling will still take place for others) a vector of numerical values corresponding to the the Plus and Minus strand scaling values respectively.
+Example:
+c{ "RNA-seq"=c(500,400) , "TT-seq"=c(1000,1000) }</t>
+  </si>
+  <si>
+    <t>check whether some datasets can indeed be left out.</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the font size for the sequencing tracks scales.</t>
+  </si>
+  <si>
+    <t>Can be "auto" or a numerical. Specify the width in cm to allocate to the tracks scale</t>
+  </si>
+  <si>
+    <t>we will also nee to report the exact formula of the size</t>
+  </si>
+  <si>
+    <t>Color as text or hex to use for the tracks scale</t>
+  </si>
+  <si>
+    <t>Title to give to the plot</t>
+  </si>
+  <si>
+    <t>Logical specifying whether the header of the plot should be displayed (TRUE) or not (FALSE)</t>
+  </si>
+  <si>
+    <t>Numerical value specifying the font size to use for the header</t>
+  </si>
+  <si>
+    <t>Vector of three colors as text or hex defining the hues to use for the Title, Subtitle (genomic coordinates) and Genomic scale texts respectively</t>
+  </si>
+  <si>
+    <t>Logical value specifying whether the genomic scale should be included (TRUE) or not (FALSE)</t>
+  </si>
+  <si>
+    <t>Logical defining whether the genomic scale should be displayed on top (TURE) or at the botom (FALSE) of the display</t>
+  </si>
+  <si>
+    <t>Numerical value defining the font size to use for the genomic scale</t>
+  </si>
+  <si>
+    <t>Logical specifying whether Features names should be displayed (TRUE) or not (FALSE)</t>
+  </si>
+  <si>
+    <t>Logical specifying whether Features names should be displayed above (TRUE) or below (FALSE) the features representation</t>
+  </si>
+  <si>
+    <t>Logical specifying whether Features names should be displayed on the opposite side of features between the Plus and minus strands</t>
+  </si>
+  <si>
+    <t>Numerical value defining the font size to use for the genomic features</t>
+  </si>
+  <si>
+    <t>Logical specifying whether Features hilighthing arrows should be displayed (TRUE) or not (FALSE)</t>
+  </si>
+  <si>
+    <t>Logical specifying whether Features hilighthing alternating colors should be displayed (TRUE) or not (FALSE)</t>
+  </si>
+  <si>
+    <t>Vector of two colors as text or hex defining the hues to use for the alternating Features highlighting colors</t>
+  </si>
+  <si>
+    <t>Numerical value defining the alpha of the Features highlighting colors</t>
+  </si>
+  <si>
+    <t>Logical specifying whether, upon usage of a unique name for all variants of a feature ("squished", "collapsed" or "collapsed2" values for the annotation_packing parameter)‚ this ame should be centered at the midle of the merged locus (FALSE) or at the center of the most dense area in features variants (TRUE)</t>
+  </si>
+  <si>
+    <t>Color as text or hex defining the hue to use for the genomic scale</t>
+  </si>
+  <si>
+    <t>Color as text or hex defining the hue to use for Features names</t>
+  </si>
+  <si>
+    <t>Logical defining whether the plot should be made as a "dummy" that des not contain sequencing data (TRUE) or not (FALSE)</t>
+  </si>
+  <si>
+    <t>Logical defining whether the plot should be disaplyed (FALSE) or saved as PDF (TRUE)</t>
+  </si>
+  <si>
+    <t>Name to use for the PDF file saving</t>
+  </si>
+  <si>
+    <t>Path to the directory to use for PDF saving</t>
+  </si>
+  <si>
+    <t>Numerical value defining a ratio to apply to the whole plot between onscreen display and PDF file saving</t>
+  </si>
+  <si>
+    <t>Can be "off", "no warnings", "normal" or "detailed". Specify the amount of information returned during the plotting.</t>
+  </si>
+  <si>
+    <t>No argument: Provides the path to the folder containing Example samples sheets</t>
+  </si>
+  <si>
+    <t>No arguement. Provides a list of the Example Sample Sheets availalble.</t>
+  </si>
+  <si>
+    <t>Helper already made</t>
+  </si>
+  <si>
+    <t>Helper aready made</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>seqNdisplayRSession object</t>
+  </si>
+  <si>
+    <t>path to save the excel including its name</t>
+  </si>
+  <si>
+    <t>No Argument. Runs the SeqNdisplay shiny App.</t>
   </si>
 </sst>
 </file>
@@ -1024,17 +1421,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1349,703 +1757,1371 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC518BC-A51B-DC4D-B368-A79657EB9F17}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D2CE25-31B8-A143-A349-99B68152E3A3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F2DE58-A45F-5C41-B18F-BDA71D49104B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F57766-25B2-CE41-8C99-2258CA8DF389}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDF5DFD-EECC-4140-A992-CB8EFB80D1E4}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FEE370-B874-3C4C-A3B1-75C82168C5AD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107E726D-875F-1047-99A7-53105977CEB9}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="197.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="197.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="87" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="88" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="208" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="208" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="2" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
+    <row r="22" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2" t="b">
+    <row r="23" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="221" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="3">
+        <v>250</v>
+      </c>
+      <c r="E31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2" t="b">
+    <row r="43" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="119" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2" t="s">
+    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D55" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2" t="b">
+      <c r="E57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D65" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="b">
+    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D66" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2" t="b">
+    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D69" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2" t="b">
+    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D70" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="b">
+    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D71" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="2" t="s">
+    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="2" t="s">
+    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D73" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D74" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D76" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D77" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D79" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D80" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="2">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="2">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>39</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47" s="2" t="b">
+    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D83" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>47</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>50</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>53</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>54</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>55</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>56</v>
-      </c>
-      <c r="D62" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>57</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>58</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>59</v>
-      </c>
-      <c r="D65" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>60</v>
-      </c>
-      <c r="D66" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>61</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>62</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>64</v>
-      </c>
-      <c r="D70" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>65</v>
-      </c>
-      <c r="D71" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>66</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>67</v>
-      </c>
-      <c r="D73" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>68</v>
-      </c>
-      <c r="D74" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>69</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>70</v>
-      </c>
-      <c r="D76" s="2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>71</v>
-      </c>
-      <c r="D77" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>72</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>73</v>
-      </c>
-      <c r="D79" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>74</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>75</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>76</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>77</v>
-      </c>
-      <c r="D83" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="B84" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="B85" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B44:B45"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C737F349-D4A2-AB44-B2AD-F257424F505A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>